<commit_message>
references and paraphrasing left
</commit_message>
<xml_diff>
--- a/Section 1/Competitor Landscape Examination/Competitor Landscape Examination Analysis.xlsx
+++ b/Section 1/Competitor Landscape Examination/Competitor Landscape Examination Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DONKAMS\Downloads\Apple_Intl_Marketing_Evaluation\Section 1\Competitor Landscape Examination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB173D7-FF90-4065-B098-94C4137984A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B7C10B-E2D6-487F-BFF8-C19E574B3BFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,54 +156,6 @@
   <dxfs count="8">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -326,13 +278,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -345,6 +290,61 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1363,13 +1363,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47EDCB04-5904-4822-9725-B3B6E69A05F8}" name="Table1" displayName="Table1" ref="A1:D6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="6" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47EDCB04-5904-4822-9725-B3B6E69A05F8}" name="Table1" displayName="Table1" ref="A1:D6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
   <autoFilter ref="A1:D6" xr:uid="{E7CC7408-0FAF-4F8D-BD9A-BAAEB3DEBC1C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1AF6D491-48BD-4DA2-9F36-DFE614D24B0B}" name="Competitor" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{57B2775B-D4FA-4700-B01E-DE574A325881}" name="Strategy Score (out of 10)" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{7EB14E29-DA66-4DD6-A4B4-FCE312B90963}" name="Brand Positioning Score (out of 10)" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{3D746C4D-0C5B-470D-ADDE-22492E32CB6B}" name="Customer Loyalty Score (out of 10)" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{1AF6D491-48BD-4DA2-9F36-DFE614D24B0B}" name="Competitor" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{57B2775B-D4FA-4700-B01E-DE574A325881}" name="Strategy Score (out of 10)" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{7EB14E29-DA66-4DD6-A4B4-FCE312B90963}" name="Brand Positioning Score (out of 10)" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{3D746C4D-0C5B-470D-ADDE-22492E32CB6B}" name="Customer Loyalty Score (out of 10)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1641,7 +1641,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>